<commit_message>
input xlsx test case
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\My Drive\clab_pypsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085ACE2F-0B96-46C0-B78E-54A07B742972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF5D165-8DE7-4B09-9E5B-E13BC48D35B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="91">
   <si>
     <t>MEM case input file</t>
   </si>
@@ -193,9 +193,6 @@
     <t>natgas</t>
   </si>
   <si>
-    <t>storage_unit</t>
-  </si>
-  <si>
     <t>battery</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
     <t>cyclic_state_of_charge</t>
   </si>
   <si>
-    <t>link</t>
-  </si>
-  <si>
     <t>electrolysis</t>
   </si>
   <si>
@@ -232,9 +226,6 @@
     <t>h2</t>
   </si>
   <si>
-    <t>store</t>
-  </si>
-  <si>
     <t>h2_storage</t>
   </si>
   <si>
@@ -281,6 +272,27 @@
   </si>
   <si>
     <t>2016-12-31 23:00:00</t>
+  </si>
+  <si>
+    <t>generators</t>
+  </si>
+  <si>
+    <t>loads</t>
+  </si>
+  <si>
+    <t>storage_units</t>
+  </si>
+  <si>
+    <t>links</t>
+  </si>
+  <si>
+    <t>stores</t>
+  </si>
+  <si>
+    <t>component_class</t>
+  </si>
+  <si>
+    <t>END_TECH_DATA</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1181,7 @@
   <dimension ref="A1:R70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,10 +1323,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1322,7 +1334,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1330,34 +1342,34 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1428,7 +1440,7 @@
     </row>
     <row r="41" spans="1:18" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>47</v>
@@ -1437,7 +1449,7 @@
         <v>48</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>15</v>
@@ -1458,7 +1470,7 @@
         <v>52</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N41" s="3" t="s">
         <v>35</v>
@@ -1469,7 +1481,7 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
         <v>55</v>
@@ -1485,18 +1497,18 @@
         <v>1.9487999999999998E-2</v>
       </c>
       <c r="I42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J42">
         <v>0</v>
       </c>
       <c r="K42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="B43" t="s">
         <v>45</v>
@@ -1513,10 +1525,10 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C44" t="s">
         <v>48</v>
@@ -1527,12 +1539,12 @@
         <v>10</v>
       </c>
       <c r="K44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
         <v>56</v>
@@ -1546,21 +1558,21 @@
         <v>1.1816999999999999E-2</v>
       </c>
       <c r="I45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J45">
         <v>3.8991999999999999E-2</v>
       </c>
       <c r="K45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" t="s">
         <v>57</v>
-      </c>
-      <c r="B46" t="s">
-        <v>58</v>
       </c>
       <c r="C46" t="s">
         <v>48</v>
@@ -1571,13 +1583,13 @@
         <v>2.541384E-2</v>
       </c>
       <c r="I46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J46">
         <v>0</v>
       </c>
       <c r="K46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L46">
         <v>6.008</v>
@@ -1592,18 +1604,18 @@
         <v>1.1400000000000001E-6</v>
       </c>
       <c r="P46" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="R46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
         <v>48</v>
@@ -1614,21 +1626,21 @@
         <v>6.4625000000000002E-2</v>
       </c>
       <c r="I47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J47">
         <v>2.2838000000000001E-2</v>
       </c>
       <c r="K47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
         <v>48</v>
@@ -1641,27 +1653,27 @@
         <v>2.0605999999999999E-2</v>
       </c>
       <c r="I48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J48">
         <v>0</v>
       </c>
       <c r="K48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C49" t="s">
         <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -1669,13 +1681,13 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J49">
         <v>0</v>
       </c>
       <c r="K49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N49">
         <v>0.7</v>
@@ -1683,13 +1695,13 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -1697,13 +1709,13 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="I50" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J50">
         <v>0</v>
       </c>
       <c r="K50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M50" t="b">
         <v>1</v>
@@ -1711,13 +1723,13 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D51" t="s">
         <v>48</v>
@@ -1726,13 +1738,13 @@
         <v>2E-3</v>
       </c>
       <c r="I51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J51">
         <v>0</v>
       </c>
       <c r="K51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N51">
         <v>0.5</v>
@@ -1740,7 +1752,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -1926,7 +1938,7 @@
         <v>40</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>48</v>
@@ -2001,7 +2013,7 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change to singule component
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\My Drive\clab_pypsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF5D165-8DE7-4B09-9E5B-E13BC48D35B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A071B0-084C-45D0-AD58-238B86A1A607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_intermodel_one_node_" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="88">
   <si>
     <t>MEM case input file</t>
   </si>
@@ -274,25 +274,16 @@
     <t>2016-12-31 23:00:00</t>
   </si>
   <si>
-    <t>generators</t>
-  </si>
-  <si>
-    <t>loads</t>
-  </si>
-  <si>
-    <t>storage_units</t>
-  </si>
-  <si>
-    <t>links</t>
-  </si>
-  <si>
-    <t>stores</t>
-  </si>
-  <si>
-    <t>component_class</t>
-  </si>
-  <si>
     <t>END_TECH_DATA</t>
+  </si>
+  <si>
+    <t>storage_unit</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>store</t>
   </si>
 </sst>
 </file>
@@ -1180,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,7 +1431,7 @@
     </row>
     <row r="41" spans="1:18" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>47</v>
@@ -1481,7 +1472,7 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
         <v>55</v>
@@ -1508,7 +1499,7 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
         <v>45</v>
@@ -1525,7 +1516,7 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="B44" t="s">
         <v>70</v>
@@ -1544,7 +1535,7 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="B45" t="s">
         <v>56</v>
@@ -1569,7 +1560,7 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
         <v>57</v>
@@ -1580,6 +1571,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="H46">
+        <f>H65*L46</f>
         <v>2.541384E-2</v>
       </c>
       <c r="I46" t="s">
@@ -1612,7 +1604,7 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="B47" t="s">
         <v>62</v>
@@ -1637,7 +1629,7 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="B48" t="s">
         <v>63</v>
@@ -1664,7 +1656,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
         <v>65</v>
@@ -1695,7 +1687,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
         <v>68</v>
@@ -1723,7 +1715,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B51" t="s">
         <v>69</v>
@@ -1752,7 +1744,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
minor change to test_case.xlsx
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\My Drive\clab_pypsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A071B0-084C-45D0-AD58-238B86A1A607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9F2A59-49D9-4C99-937F-18C86342BFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="90">
   <si>
     <t>MEM case input file</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t>store</t>
+  </si>
+  <si>
+    <t>Note that any information that is in a column without an attribute header is consider a comment, and not used.</t>
+  </si>
+  <si>
+    <t>Note that cell H46 contains a formula, and our PyPSA front end will read this in as a value.</t>
   </si>
 </sst>
 </file>
@@ -788,7 +794,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -803,7 +809,6 @@
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -814,6 +819,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1169,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R70"/>
+  <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,7 +1358,7 @@
       <c r="A30" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>81</v>
       </c>
       <c r="C30" t="s">
@@ -1359,18 +1369,18 @@
       <c r="A31" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="13" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="12"/>
+      <c r="B32" s="11"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="13" t="b">
+      <c r="B33" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1570,8 +1580,8 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="H46">
-        <f>H65*L46</f>
+      <c r="H46" s="5">
+        <f>H64*L46</f>
         <v>2.541384E-2</v>
       </c>
       <c r="I46" t="s">
@@ -1747,266 +1757,248 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9" t="s">
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H59" s="9" t="s">
+      <c r="H59" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I59" s="9" t="s">
+      <c r="I59" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J59" s="9" t="s">
+      <c r="J59" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K59" s="10" t="s">
+      <c r="K59" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="L59" s="10" t="s">
+      <c r="L59" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-      <c r="L60" s="11"/>
-    </row>
-    <row r="61" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I60" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J60" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K60" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L60" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>48</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F61" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G61" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H61" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I61" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="J61" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="K61" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="L61" s="10" t="s">
-        <v>54</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10">
+        <v>1.9487999999999998E-2</v>
+      </c>
+      <c r="I61" s="10">
+        <v>0</v>
+      </c>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F62" s="10">
+        <v>1</v>
+      </c>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="10"/>
+      <c r="K62" s="10"/>
+      <c r="L62" s="10"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C62" s="11" t="s">
+      <c r="B63" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D62" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11">
-        <v>1.9487999999999998E-2</v>
-      </c>
-      <c r="I62" s="11">
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10">
+        <v>1.1816999999999999E-2</v>
+      </c>
+      <c r="I63" s="10">
+        <v>3.8991999999999999E-2</v>
+      </c>
+      <c r="J63" s="10"/>
+      <c r="K63" s="10"/>
+      <c r="L63" s="10"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10">
+        <v>4.2300000000000003E-3</v>
+      </c>
+      <c r="I64" s="10">
         <v>0</v>
       </c>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
-      <c r="L62" s="11"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E63" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F63" s="11">
-        <v>1</v>
-      </c>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="11"/>
-      <c r="K63" s="11"/>
-      <c r="L63" s="11"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11">
-        <v>1.1816999999999999E-2</v>
-      </c>
-      <c r="I64" s="11">
-        <v>3.8991999999999999E-2</v>
-      </c>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
-      <c r="L64" s="11"/>
+      <c r="J64" s="10">
+        <v>6.008</v>
+      </c>
+      <c r="K64" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="L64" s="10">
+        <v>1.1400000000000001E-6</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B65" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11">
-        <v>4.2300000000000003E-3</v>
-      </c>
-      <c r="I65" s="11">
+      <c r="A65" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10">
+        <v>6.4625000000000002E-2</v>
+      </c>
+      <c r="I65" s="10">
+        <v>2.2838000000000001E-2</v>
+      </c>
+      <c r="J65" s="10"/>
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10">
+        <v>2.0605999999999999E-2</v>
+      </c>
+      <c r="I66" s="10">
         <v>0</v>
       </c>
-      <c r="J65" s="11">
-        <v>6.008</v>
-      </c>
-      <c r="K65" s="11">
-        <v>0.9</v>
-      </c>
-      <c r="L65" s="11">
-        <v>1.1400000000000001E-6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11">
-        <v>6.4625000000000002E-2</v>
-      </c>
-      <c r="I66" s="11">
-        <v>2.2838000000000001E-2</v>
-      </c>
-      <c r="J66" s="11"/>
-      <c r="K66" s="11"/>
-      <c r="L66" s="11"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E67" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11">
-        <v>2.0605999999999999E-2</v>
-      </c>
-      <c r="I67" s="11">
-        <v>0</v>
-      </c>
-      <c r="J67" s="11"/>
-      <c r="K67" s="11"/>
-      <c r="L67" s="11"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
+      <c r="L66" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Including commits from master
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\My Drive\clab_pypsa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_pypsa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9F2A59-49D9-4C99-937F-18C86342BFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993F836B-BBFD-2749-88BE-F2028AE51F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_intermodel_one_node_" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="96">
   <si>
     <t>MEM case input file</t>
   </si>
@@ -112,9 +126,6 @@
     <t>output_path</t>
   </si>
   <si>
-    <t>verbose</t>
-  </si>
-  <si>
     <t>numerics_scaling</t>
   </si>
   <si>
@@ -232,9 +243,6 @@
     <t>fuel_cell</t>
   </si>
   <si>
-    <t>lost_load</t>
-  </si>
-  <si>
     <t>$/h/kWh</t>
   </si>
   <si>
@@ -290,6 +298,30 @@
   </si>
   <si>
     <t>Note that cell H46 contains a formula, and our PyPSA front end will read this in as a value.</t>
+  </si>
+  <si>
+    <t>logging_level</t>
+  </si>
+  <si>
+    <t>warning</t>
+  </si>
+  <si>
+    <t>Note: Can be error, warning, info, or debug</t>
+  </si>
+  <si>
+    <t>solar.csv</t>
+  </si>
+  <si>
+    <t>demand.csv</t>
+  </si>
+  <si>
+    <t>wind.csv</t>
+  </si>
+  <si>
+    <t>time_series_file</t>
+  </si>
+  <si>
+    <t>time_steps</t>
   </si>
 </sst>
 </file>
@@ -794,7 +826,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -819,11 +851,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1181,58 +1212,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A45" activeCellId="3" sqref="A51:XFD51 A52:XFD52 A50:XFD50 A45:XFD45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="4" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="22.28515625" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="14" max="14" width="11.5" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="16" max="16" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1240,7 +1272,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1248,12 +1280,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1261,7 +1293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1269,7 +1301,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1277,7 +1309,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1285,7 +1317,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1293,7 +1325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1301,7 +1333,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1309,7 +1341,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1317,281 +1349,272 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>73</v>
       </c>
-      <c r="B29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="13" t="s">
+      <c r="B31" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="11"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="15">
+        <f>(B31-B30)*24+1</f>
+        <v>8784.0000000000582</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B33" s="11"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B35" s="1">
+        <v>9.9999999999999998E+23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O40" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="1">
-        <v>9.9999999999999998E+23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    </row>
+    <row r="42" spans="1:18" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O42" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="H43">
+        <f>H58*B32</f>
+        <v>171.18259200000111</v>
+      </c>
+      <c r="I43" t="s">
+        <v>58</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L39" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N39" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="O39" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="3" t="s">
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L41" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="M41" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="N41" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O41" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="E44" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" t="s">
         <v>55</v>
       </c>
-      <c r="C42" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F42" s="2"/>
-      <c r="H42">
-        <v>1.9487999999999998E-2</v>
-      </c>
-      <c r="I42" t="s">
-        <v>59</v>
-      </c>
-      <c r="J42">
-        <v>0</v>
-      </c>
-      <c r="K42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F43" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" t="s">
-        <v>48</v>
-      </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="J44">
-        <v>10</v>
-      </c>
-      <c r="K44" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" t="s">
-        <v>56</v>
-      </c>
       <c r="C45" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" s="2"/>
+        <v>47</v>
+      </c>
       <c r="F45" s="2"/>
       <c r="H45">
-        <v>1.1816999999999999E-2</v>
+        <f>H60*B32</f>
+        <v>103.80052800000068</v>
       </c>
       <c r="I45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J45">
         <v>3.8991999999999999E-2</v>
       </c>
       <c r="K45" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" t="s">
-        <v>48</v>
-      </c>
-      <c r="E46" s="2"/>
+        <v>47</v>
+      </c>
       <c r="F46" s="2"/>
       <c r="H46" s="5">
-        <f>H64*L46</f>
-        <v>2.541384E-2</v>
+        <f>H61*L46*B32</f>
+        <v>223.23517056000148</v>
       </c>
       <c r="I46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J46">
         <v>0</v>
       </c>
       <c r="K46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L46">
         <v>6.008</v>
@@ -1606,398 +1629,399 @@
         <v>1.1400000000000001E-6</v>
       </c>
       <c r="P46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>39</v>
-      </c>
-      <c r="B47" t="s">
-        <v>62</v>
-      </c>
       <c r="C47" t="s">
-        <v>48</v>
-      </c>
-      <c r="E47" s="2"/>
+        <v>47</v>
+      </c>
       <c r="F47" s="2"/>
       <c r="H47">
-        <v>6.4625000000000002E-2</v>
+        <f>H62*B32</f>
+        <v>567.66600000000381</v>
       </c>
       <c r="I47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J47">
         <v>2.2838000000000001E-2</v>
       </c>
       <c r="K47" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>48</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="E48" t="s">
+        <v>93</v>
       </c>
       <c r="F48" s="2"/>
       <c r="H48">
-        <v>2.0605999999999999E-2</v>
+        <f>H63*B32</f>
+        <v>181.0031040000012</v>
       </c>
       <c r="I48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J48">
         <v>0</v>
       </c>
       <c r="K48" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>86</v>
       </c>
-      <c r="B49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" t="s">
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>87</v>
+      </c>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+    </row>
+    <row r="56" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K56" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L56" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A57" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G57" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D49" t="s">
-        <v>67</v>
-      </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="H49">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="I49" t="s">
-        <v>59</v>
-      </c>
-      <c r="J49">
+      <c r="H57" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K57" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L57" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10">
+        <v>1.9487999999999998E-2</v>
+      </c>
+      <c r="I58" s="10">
         <v>0</v>
       </c>
-      <c r="K49" t="s">
-        <v>60</v>
-      </c>
-      <c r="N49">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" t="s">
-        <v>67</v>
-      </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="H50">
-        <v>1.5999999999999999E-5</v>
-      </c>
-      <c r="I50" t="s">
-        <v>71</v>
-      </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
-      <c r="K50" t="s">
-        <v>60</v>
-      </c>
-      <c r="M50" t="b">
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F59" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>86</v>
-      </c>
-      <c r="B51" t="s">
-        <v>69</v>
-      </c>
-      <c r="C51" t="s">
-        <v>67</v>
-      </c>
-      <c r="D51" t="s">
-        <v>48</v>
-      </c>
-      <c r="H51">
-        <v>2E-3</v>
-      </c>
-      <c r="I51" t="s">
-        <v>59</v>
-      </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
-      <c r="K51" t="s">
-        <v>60</v>
-      </c>
-      <c r="N51">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="K57" s="16"/>
-      <c r="L57" s="16"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H59" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I59" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J59" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K59" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="L59" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B60" s="9" t="s">
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C60" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I60" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J60" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="K60" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="L60" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10">
+        <v>1.1816999999999999E-2</v>
+      </c>
+      <c r="I60" s="10">
+        <v>3.8991999999999999E-2</v>
+      </c>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>37</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
       <c r="H61" s="10">
-        <v>1.9487999999999998E-2</v>
+        <v>4.2300000000000003E-3</v>
       </c>
       <c r="I61" s="10">
         <v>0</v>
       </c>
-      <c r="J61" s="10"/>
-      <c r="K61" s="10"/>
-      <c r="L61" s="10"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J61" s="10">
+        <v>6.008</v>
+      </c>
+      <c r="K61" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="L61" s="10">
+        <v>1.1400000000000001E-6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F62" s="10">
-        <v>1</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
       <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
-      <c r="I62" s="10"/>
+      <c r="H62" s="10">
+        <v>6.4625000000000002E-2</v>
+      </c>
+      <c r="I62" s="10">
+        <v>2.2838000000000001E-2</v>
+      </c>
       <c r="J62" s="10"/>
       <c r="K62" s="10"/>
       <c r="L62" s="10"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
+        <v>41</v>
+      </c>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
       <c r="H63" s="10">
-        <v>1.1816999999999999E-2</v>
+        <v>2.0605999999999999E-2</v>
       </c>
       <c r="I63" s="10">
-        <v>3.8991999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="J63" s="10"/>
       <c r="K63" s="10"/>
       <c r="L63" s="10"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D64" s="10"/>
+        <v>47</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="E64" s="10"/>
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
       <c r="H64" s="10">
-        <v>4.2300000000000003E-3</v>
-      </c>
-      <c r="I64" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J64" s="10">
         <v>0</v>
       </c>
-      <c r="J64" s="10">
-        <v>6.008</v>
-      </c>
-      <c r="K64" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="L64" s="10">
-        <v>1.1400000000000001E-6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K64" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L64" s="10"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C65" s="10"/>
+        <v>67</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
       <c r="H65" s="10">
-        <v>6.4625000000000002E-2</v>
-      </c>
-      <c r="I65" s="10">
-        <v>2.2838000000000001E-2</v>
-      </c>
-      <c r="J65" s="10"/>
-      <c r="K65" s="10"/>
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J65" s="10">
+        <v>0</v>
+      </c>
+      <c r="K65" s="10" t="s">
+        <v>59</v>
+      </c>
       <c r="L65" s="10"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C66" s="10"/>
+        <v>68</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="D66" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E66" s="10" t="s">
-        <v>43</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E66" s="10"/>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
       <c r="H66" s="10">
-        <v>2.0605999999999999E-2</v>
-      </c>
-      <c r="I66" s="10">
+        <v>2E-3</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J66" s="10">
         <v>0</v>
       </c>
-      <c r="J66" s="10"/>
-      <c r="K66" s="10"/>
+      <c r="K66" s="10" t="s">
+        <v>59</v>
+      </c>
       <c r="L66" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simple fix scaling, rename tech->component
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_pypsa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515BF258-7A7D-1745-B7AD-BB2F3EBD17A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD98C95-54D5-0849-9963-80C85B3DF19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="4580" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="500" windowWidth="27920" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_intermodel_one_node_" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="107">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -80,9 +80,6 @@
     <t>numerics_scaling</t>
   </si>
   <si>
-    <t>TECH_DATA</t>
-  </si>
-  <si>
     <t>normalization</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>Note that for MEM, storage is in energy units whereas for PyPSA it is in power units.</t>
   </si>
   <si>
-    <t>$/h/kW</t>
-  </si>
-  <si>
     <t>Note: PyPSA costs storage_unit by power cost; cost of energy capacity is effectively capital_cost/max_hours</t>
   </si>
   <si>
@@ -149,9 +143,21 @@
     <t>cyclic_state_of_charge</t>
   </si>
   <si>
+    <t>electrolysis</t>
+  </si>
+  <si>
     <t>bus1</t>
   </si>
   <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>h2_storage</t>
+  </si>
+  <si>
+    <t>fuel_cell</t>
+  </si>
+  <si>
     <t>filename_prefix</t>
   </si>
   <si>
@@ -164,18 +170,12 @@
     <t>output_data</t>
   </si>
   <si>
-    <t>input_data</t>
-  </si>
-  <si>
     <t>input_path</t>
   </si>
   <si>
     <t>Note: Dates must be formatted as text (not excel date format)</t>
   </si>
   <si>
-    <t>END_TECH_DATA</t>
-  </si>
-  <si>
     <t>Note that any information that is in a column without an attribute header is consider a comment, and not used.</t>
   </si>
   <si>
@@ -206,9 +206,6 @@
     <t>Load</t>
   </si>
   <si>
-    <t>#Generator</t>
-  </si>
-  <si>
     <t>StorageUnit</t>
   </si>
   <si>
@@ -227,9 +224,6 @@
     <t>PyPSA case input file</t>
   </si>
   <si>
-    <t>Everything outside of  the &lt;CASE&gt; or &lt;TECH&gt;  flag is for notes, etc.</t>
-  </si>
-  <si>
     <t>PyPSA component type</t>
   </si>
   <si>
@@ -317,25 +311,49 @@
     <t>delta_t</t>
   </si>
   <si>
-    <t>time_range</t>
-  </si>
-  <si>
     <t>Note: Capital costs are the product of hourly fixed costs and time_range</t>
   </si>
   <si>
     <t>Note: This is a test case, the costs aren't meant to be very realistic but provide reproducibility in tests</t>
   </si>
   <si>
-    <t>2016-01-01 01:00:00</t>
-  </si>
-  <si>
     <t>2017-01-01 0:00:00</t>
   </si>
   <si>
-    <t>test_case_solar</t>
-  </si>
-  <si>
-    <t>test_prefix_solar_noscaling</t>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Note: this assumes time unit for dt is 'hour'</t>
+  </si>
+  <si>
+    <t>2016-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>no_time_steps</t>
+  </si>
+  <si>
+    <t>total_hours</t>
+  </si>
+  <si>
+    <t>Everything outside of  the &lt;CASE_DATA&gt; or &lt;COMPONENT_DATA&gt;  flag is for notes, etc.</t>
+  </si>
+  <si>
+    <t>COMPONENT_DATA</t>
+  </si>
+  <si>
+    <t>END_COMPONENT_DATA</t>
+  </si>
+  <si>
+    <t>test_prefix</t>
+  </si>
+  <si>
+    <t>test_case</t>
+  </si>
+  <si>
+    <t>/carnegie/data/Shared/Labs/Caldeira\ Lab/Everyone/energy_demand_capacity_data/test_case_solar_wind_demand/</t>
   </si>
 </sst>
 </file>
@@ -345,7 +363,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,6 +505,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="36">
@@ -866,7 +889,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -902,7 +925,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1258,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S69"/>
+  <dimension ref="A1:S76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1285,7 +1310,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1303,7 +1328,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1341,7 +1366,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1369,10 +1394,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1381,10 +1406,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1393,10 +1418,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1426,7 +1451,7 @@
         <v>53</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1435,10 +1460,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1447,10 +1472,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1459,10 +1484,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1471,10 +1496,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1483,10 +1508,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1495,10 +1520,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1512,10 +1537,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1523,7 +1548,7 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1531,354 +1556,317 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C30" s="8"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B31">
-        <f>INT((B30-B29)*24+1)</f>
+        <v>1</v>
+      </c>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="21">
+        <f>(B30-B29)*24/B31</f>
         <v>8784</v>
       </c>
-      <c r="C31" s="10"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="10"/>
+      <c r="C32" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+      <c r="A33" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" s="21">
+        <f>B32*B31</f>
+        <v>8784</v>
+      </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" t="s">
-        <v>60</v>
-      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="1">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="D35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B36" s="1"/>
+      <c r="B36" s="1">
+        <v>10000000000</v>
+      </c>
       <c r="C36" s="1"/>
+      <c r="D36" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B40" s="1"/>
+      <c r="A40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>19</v>
-      </c>
-      <c r="I41" t="s">
-        <v>95</v>
-      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D42" t="s">
-        <v>78</v>
-      </c>
-      <c r="H42" t="s">
-        <v>85</v>
-      </c>
-      <c r="O42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>76</v>
+      </c>
+      <c r="H43" t="s">
+        <v>83</v>
+      </c>
+      <c r="O43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="G45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="I45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O45" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="M44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="O44" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5" t="s">
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="H47" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H46" s="2" t="s">
+      <c r="I47" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="K47" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="M47" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M46" s="2" t="s">
+      <c r="N47" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q47" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="N46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O46" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" t="s">
-        <v>29</v>
-      </c>
-      <c r="D47" t="s">
-        <v>23</v>
-      </c>
-      <c r="F47" t="s">
-        <v>50</v>
-      </c>
-      <c r="I47" s="15">
-        <f>L64*B31</f>
-        <v>171.65443408509168</v>
-      </c>
-      <c r="J47" t="str">
-        <f>B39 &amp; "/time range/" &amp; B38</f>
-        <v>$/time range/kW</v>
-      </c>
-      <c r="K47" s="15">
-        <v>0</v>
-      </c>
-      <c r="L47" t="str">
-        <f xml:space="preserve"> B39 &amp; "/" &amp; B38 &amp; B37</f>
-        <v>$/kWh</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C48" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F48" t="s">
-        <v>51</v>
-      </c>
-      <c r="I48" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="I48" s="21">
+        <f>L68*B33</f>
+        <v>171.65443408509168</v>
+      </c>
+      <c r="J48" t="str">
+        <f>B40 &amp; "/time range/" &amp; B39</f>
+        <v>$/time range/kW</v>
+      </c>
       <c r="K48" s="15"/>
+      <c r="L48" t="str">
+        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+        <v>$/kWh</v>
+      </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C49" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D49" t="s">
-        <v>23</v>
-      </c>
-      <c r="I49" s="15">
-        <f>L65*B31</f>
-        <v>104.08824719790415</v>
-      </c>
-      <c r="J49" t="str">
-        <f>B39 &amp; "/time range/" &amp; B38</f>
-        <v>$/time range/kW</v>
-      </c>
-      <c r="K49" s="15">
-        <f>H65 + I65/J65</f>
-        <v>3.9088110924995347E-2</v>
-      </c>
-      <c r="L49" t="str">
-        <f xml:space="preserve"> B39 &amp; "/" &amp; B38 &amp; B37</f>
-        <v>$/kWh</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F49" t="s">
+        <v>51</v>
+      </c>
+      <c r="I49" s="15"/>
+      <c r="K49" s="15"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D50" t="s">
-        <v>23</v>
-      </c>
-      <c r="I50" s="15">
-        <f>L66*M50*B31</f>
-        <v>223.87212597208145</v>
+        <v>22</v>
+      </c>
+      <c r="I50" s="21">
+        <f>L69*B33</f>
+        <v>104.08824719790415</v>
       </c>
       <c r="J50" t="str">
-        <f>B39 &amp; "/time range/" &amp; B38</f>
+        <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K50" s="15"/>
+      <c r="K50" s="15">
+        <f>H69 + I69/J69</f>
+        <v>3.9088110924995347E-2</v>
+      </c>
       <c r="L50" t="str">
-        <f xml:space="preserve"> B39 &amp; "/" &amp; B38 &amp; B37</f>
+        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
-      </c>
-      <c r="M50">
-        <v>6.008</v>
-      </c>
-      <c r="N50" t="b">
-        <v>1</v>
-      </c>
-      <c r="O50">
-        <v>0.9</v>
-      </c>
-      <c r="Q50">
-        <v>1.1400000000000001E-6</v>
-      </c>
-      <c r="R50" t="str">
-        <f xml:space="preserve"> 1 &amp; "/" &amp; B37</f>
-        <v>1/h</v>
-      </c>
-      <c r="S50" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
@@ -1886,327 +1874,319 @@
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D51" t="s">
-        <v>23</v>
-      </c>
-      <c r="I51" s="15">
-        <f>L67*B31</f>
-        <v>548.78374889246641</v>
+        <v>22</v>
+      </c>
+      <c r="I51" s="21">
+        <f>L70*M51*B33</f>
+        <v>223.87212597208145</v>
       </c>
       <c r="J51" t="str">
-        <f>B39 &amp; "/time range/" &amp; B38</f>
+        <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K51" s="15">
-        <f t="shared" ref="K50:K51" si="0">H67 + I67/J67</f>
-        <v>2.5047272727272724E-2</v>
-      </c>
+      <c r="K51" s="15"/>
       <c r="L51" t="str">
-        <f xml:space="preserve"> B39 &amp; "/" &amp; B38 &amp; B37</f>
+        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
+      </c>
+      <c r="M51">
+        <v>6.008</v>
+      </c>
+      <c r="N51" t="b">
+        <v>1</v>
+      </c>
+      <c r="O51">
+        <v>0.9</v>
+      </c>
+      <c r="Q51">
+        <v>1.1400000000000001E-6</v>
+      </c>
+      <c r="R51" t="str">
+        <f xml:space="preserve"> 1 &amp; "/" &amp; B38</f>
+        <v>1/h</v>
+      </c>
+      <c r="S51" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" s="21">
+        <f>L71*B33</f>
+        <v>548.78374889246641</v>
+      </c>
+      <c r="J52" t="str">
+        <f>B40 &amp; "/time range/" &amp; B39</f>
+        <v>$/time range/kW</v>
+      </c>
+      <c r="K52" s="15">
+        <f>H71 + I71/J71</f>
+        <v>2.5047272727272724E-2</v>
+      </c>
+      <c r="L52" t="str">
+        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+        <v>$/kWh</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" t="s">
+        <v>52</v>
+      </c>
+      <c r="I53" s="21">
+        <f>L72*B33</f>
+        <v>181.49756560590552</v>
+      </c>
+      <c r="J53" t="str">
+        <f>B40 &amp; "/time range/" &amp; B39</f>
+        <v>$/time range/kW</v>
+      </c>
+      <c r="K53" s="15"/>
+      <c r="L53" t="str">
+        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+        <v>$/kWh</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" t="s">
         <v>36</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>36</v>
       </c>
-      <c r="D52" t="s">
-        <v>23</v>
-      </c>
-      <c r="F52" t="s">
-        <v>52</v>
-      </c>
-      <c r="I52" s="15">
-        <f>L68*B31</f>
-        <v>181.49756560590552</v>
-      </c>
-      <c r="J52" t="str">
-        <f>B39 &amp; "/time range/" &amp; B38</f>
+      <c r="D54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54" t="s">
+        <v>38</v>
+      </c>
+      <c r="I54" s="21">
+        <f>L73*B33</f>
+        <v>43.92</v>
+      </c>
+      <c r="J54" t="str">
+        <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K52" s="15">
-        <v>0</v>
-      </c>
-      <c r="L52" t="str">
-        <f xml:space="preserve"> B39 &amp; "/" &amp; B38 &amp; B37</f>
+      <c r="K54" s="15"/>
+      <c r="L54" t="str">
+        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>46</v>
+      <c r="O54">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" t="s">
+        <v>39</v>
+      </c>
+      <c r="D55" t="s">
+        <v>38</v>
+      </c>
+      <c r="I55" s="21">
+        <f>L74*B33</f>
+        <v>0.140544</v>
+      </c>
+      <c r="J55" t="str">
+        <f>B40 &amp; "/time range/" &amp; B39 &amp; B38</f>
+        <v>$/time range/kWh</v>
+      </c>
+      <c r="K55" s="15"/>
+      <c r="L55" t="str">
+        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+        <v>$/kWh</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="A56" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B56" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" t="s">
+        <v>22</v>
+      </c>
+      <c r="I56" s="21">
+        <f>L75*B33</f>
+        <v>17.568000000000001</v>
+      </c>
+      <c r="J56" t="str">
+        <f>B40 &amp; "/time range/" &amp; B39</f>
+        <v>$/time range/kW</v>
+      </c>
+      <c r="K56" s="15"/>
+      <c r="L56" t="str">
+        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+        <v>$/kWh</v>
+      </c>
+      <c r="O56">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A58" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="L58" s="9"/>
-      <c r="M58" s="9"/>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>91</v>
-      </c>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
-    </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A61" s="12" t="s">
+      <c r="A61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A62" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>89</v>
+      </c>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A65" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" s="12"/>
+      <c r="B66" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
-      <c r="L61" s="2"/>
-      <c r="M61" s="2"/>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A62" s="12"/>
-      <c r="B62" s="16" t="s">
+      <c r="C66" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+      <c r="I66" s="16"/>
+      <c r="J66" s="16"/>
+      <c r="K66" s="16"/>
+      <c r="L66" s="16"/>
+      <c r="M66" s="16"/>
+    </row>
+    <row r="67" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A67" s="2"/>
+      <c r="B67" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" s="19" t="str">
+        <f xml:space="preserve"> "Overnight cost [" &amp; B40 &amp; "/" &amp; B39 &amp; "]"</f>
+        <v>Overnight cost [$/kW]</v>
+      </c>
+      <c r="D67" s="13" t="str">
+        <f xml:space="preserve"> "Fixed O&amp;M cost ["  &amp; B40 &amp; "/" &amp; B39 &amp; "year]"</f>
+        <v>Fixed O&amp;M cost [$/kWyear]</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G67" s="17" t="str">
+        <f xml:space="preserve"> "Annual fixed costs [" &amp;B40 &amp; "/year]"</f>
+        <v>Annual fixed costs [$/year]</v>
+      </c>
+      <c r="H67" s="13" t="str">
+        <f xml:space="preserve"> "Variable O&amp;M [" &amp; B40 &amp; "/" &amp; B39 &amp; B38 &amp; "]"</f>
+        <v>Variable O&amp;M [$/kWh]</v>
+      </c>
+      <c r="I67" s="13" t="str">
+        <f xml:space="preserve"> "Fuel cost [" &amp; B40 &amp; "/" &amp; B39 &amp; B38 &amp; "]"</f>
+        <v>Fuel cost [$/kWh]</v>
+      </c>
+      <c r="J67" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C62" s="14">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16"/>
-      <c r="I62" s="16"/>
-      <c r="J62" s="16"/>
-      <c r="K62" s="16"/>
-      <c r="L62" s="16"/>
-      <c r="M62" s="16"/>
-    </row>
-    <row r="63" spans="1:19" ht="64" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-      <c r="B63" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C63" s="19" t="str">
-        <f xml:space="preserve"> "Overnight cost [" &amp; B39 &amp; "/" &amp; B38 &amp; "]"</f>
-        <v>Overnight cost [$/kW]</v>
-      </c>
-      <c r="D63" s="13" t="str">
-        <f xml:space="preserve"> "Fixed O&amp;M cost ["  &amp; B39 &amp; "/" &amp; B38 &amp; "year]"</f>
-        <v>Fixed O&amp;M cost [$/kWyear]</v>
-      </c>
-      <c r="E63" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F63" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="G63" s="17" t="str">
-        <f xml:space="preserve"> "Annual fixed costs [" &amp;B39 &amp; "/year]"</f>
-        <v>Annual fixed costs [$/year]</v>
-      </c>
-      <c r="H63" s="13" t="str">
-        <f xml:space="preserve"> "Variable O&amp;M [" &amp; B39 &amp; "/" &amp; B38 &amp; B37 &amp; "]"</f>
-        <v>Variable O&amp;M [$/kWh]</v>
-      </c>
-      <c r="I63" s="13" t="str">
-        <f xml:space="preserve"> "Fuel cost [" &amp; B39 &amp; "/" &amp; B38 &amp; B37 &amp; "]"</f>
-        <v>Fuel cost [$/kWh]</v>
-      </c>
-      <c r="J63" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="K63" s="19"/>
-      <c r="L63" s="13" t="s">
+      <c r="K67" s="19"/>
+      <c r="L67" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="M63" s="13"/>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B64" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C64" s="20">
+      <c r="M67" s="13"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B68" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C68" s="20">
         <v>1851</v>
       </c>
-      <c r="D64" s="14">
+      <c r="D68" s="14">
         <v>22.02</v>
       </c>
-      <c r="E64" s="14">
-        <f>C62*(1+C62)^F64/((1+C62)^F64-1)</f>
-        <v>8.0586403511111196E-2</v>
-      </c>
-      <c r="F64" s="14">
-        <v>30</v>
-      </c>
-      <c r="G64" s="18">
-        <f>C64*E64+D64</f>
-        <v>171.18543289906683</v>
-      </c>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="20"/>
-      <c r="L64" s="14">
-        <f>G64/8760</f>
-        <v>1.954171608436836E-2</v>
-      </c>
-      <c r="M64" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B65" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C65" s="20">
-        <v>982</v>
-      </c>
-      <c r="D65" s="14">
-        <v>11.11</v>
-      </c>
-      <c r="E65" s="14">
-        <f>C62*(1+C62)^F65/((1+C62)^F65-1)</f>
-        <v>9.4392925743255696E-2</v>
-      </c>
-      <c r="F65" s="14">
-        <v>20</v>
-      </c>
-      <c r="G65" s="18">
-        <f>C65*E65+D65</f>
-        <v>103.80385307987709</v>
-      </c>
-      <c r="H65" s="14">
-        <v>3.5400000000000002E-3</v>
-      </c>
-      <c r="I65" s="14">
-        <v>1.9099999999999999E-2</v>
-      </c>
-      <c r="J65" s="14">
-        <v>0.5373</v>
-      </c>
-      <c r="K65" s="20"/>
-      <c r="L65" s="14">
-        <f>G65/8760</f>
-        <v>1.1849754917794188E-2</v>
-      </c>
-      <c r="M65" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B66" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C66" s="20">
-        <v>261</v>
-      </c>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14">
-        <f>C62*(1+C62)^F66/((1+C62)^F66-1)</f>
-        <v>0.14237750272736471</v>
-      </c>
-      <c r="F66" s="14">
-        <v>10</v>
-      </c>
-      <c r="G66" s="18">
-        <f>C66*E66+D66</f>
-        <v>37.160528211842191</v>
-      </c>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="20"/>
-      <c r="L66" s="14">
-        <f>G66/8760</f>
-        <v>4.2420694305755928E-3</v>
-      </c>
-      <c r="M66" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B67" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C67" s="20">
-        <v>5946</v>
-      </c>
-      <c r="D67" s="14">
-        <v>101.28</v>
-      </c>
-      <c r="E67" s="14">
-        <f>C62*(1+C62)^F67/((1+C62)^F67-1)</f>
-        <v>7.5009138873610326E-2</v>
-      </c>
-      <c r="F67" s="14">
-        <v>40</v>
-      </c>
-      <c r="G67" s="18">
-        <f>C67*E67+D67</f>
-        <v>547.28433974248696</v>
-      </c>
-      <c r="H67" s="14">
-        <v>2.32E-3</v>
-      </c>
-      <c r="I67" s="14">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="J67" s="14">
-        <v>0.33</v>
-      </c>
-      <c r="K67" s="20"/>
-      <c r="L67" s="14">
-        <f>G67/8760</f>
-        <v>6.2475381249142349E-2</v>
-      </c>
-      <c r="M67" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B68" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C68" s="20">
-        <v>1657</v>
-      </c>
-      <c r="D68" s="14">
-        <v>47.47</v>
-      </c>
       <c r="E68" s="14">
-        <f>C62*(1+C62)^F68/((1+C62)^F68-1)</f>
+        <f>C66*(1+C66)^F68/((1+C66)^F68-1)</f>
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="F68" s="14">
@@ -2214,7 +2194,7 @@
       </c>
       <c r="G68" s="18">
         <f>C68*E68+D68</f>
-        <v>181.00167061791126</v>
+        <v>171.18543289906683</v>
       </c>
       <c r="H68" s="14"/>
       <c r="I68" s="14"/>
@@ -2222,15 +2202,225 @@
       <c r="K68" s="20"/>
       <c r="L68" s="14">
         <f>G68/8760</f>
+        <v>1.954171608436836E-2</v>
+      </c>
+      <c r="M68" s="14" t="str">
+        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <v>$/h/kW</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B69" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" s="20">
+        <v>982</v>
+      </c>
+      <c r="D69" s="14">
+        <v>11.11</v>
+      </c>
+      <c r="E69" s="14">
+        <f>C66*(1+C66)^F69/((1+C66)^F69-1)</f>
+        <v>9.4392925743255696E-2</v>
+      </c>
+      <c r="F69" s="14">
+        <v>20</v>
+      </c>
+      <c r="G69" s="18">
+        <f>C69*E69+D69</f>
+        <v>103.80385307987709</v>
+      </c>
+      <c r="H69" s="14">
+        <v>3.5400000000000002E-3</v>
+      </c>
+      <c r="I69" s="14">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="J69" s="14">
+        <v>0.5373</v>
+      </c>
+      <c r="K69" s="20"/>
+      <c r="L69" s="14">
+        <f>G69/8760</f>
+        <v>1.1849754917794188E-2</v>
+      </c>
+      <c r="M69" s="14" t="str">
+        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <v>$/h/kW</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B70" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70" s="20">
+        <v>261</v>
+      </c>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14">
+        <f>C66*(1+C66)^F70/((1+C66)^F70-1)</f>
+        <v>0.14237750272736471</v>
+      </c>
+      <c r="F70" s="14">
+        <v>10</v>
+      </c>
+      <c r="G70" s="18">
+        <f>C70*E70+D70</f>
+        <v>37.160528211842191</v>
+      </c>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="14">
+        <f>G70/8760</f>
+        <v>4.2420694305755928E-3</v>
+      </c>
+      <c r="M70" s="14" t="str">
+        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <v>$/h/kW</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B71" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" s="20">
+        <v>5946</v>
+      </c>
+      <c r="D71" s="14">
+        <v>101.28</v>
+      </c>
+      <c r="E71" s="14">
+        <f>C66*(1+C66)^F71/((1+C66)^F71-1)</f>
+        <v>7.5009138873610326E-2</v>
+      </c>
+      <c r="F71" s="14">
+        <v>40</v>
+      </c>
+      <c r="G71" s="18">
+        <f>C71*E71+D71</f>
+        <v>547.28433974248696</v>
+      </c>
+      <c r="H71" s="14">
+        <v>2.32E-3</v>
+      </c>
+      <c r="I71" s="14">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="J71" s="14">
+        <v>0.33</v>
+      </c>
+      <c r="K71" s="20"/>
+      <c r="L71" s="14">
+        <f>G71/8760</f>
+        <v>6.2475381249142349E-2</v>
+      </c>
+      <c r="M71" s="14" t="str">
+        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <v>$/h/kW</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B72" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C72" s="20">
+        <v>1657</v>
+      </c>
+      <c r="D72" s="14">
+        <v>47.47</v>
+      </c>
+      <c r="E72" s="14">
+        <f>C66*(1+C66)^F72/((1+C66)^F72-1)</f>
+        <v>8.0586403511111196E-2</v>
+      </c>
+      <c r="F72" s="14">
+        <v>30</v>
+      </c>
+      <c r="G72" s="18">
+        <f>C72*E72+D72</f>
+        <v>181.00167061791126</v>
+      </c>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="20"/>
+      <c r="L72" s="14">
+        <f>G72/8760</f>
         <v>2.0662291166428225E-2</v>
       </c>
-      <c r="M68" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B69" s="21" t="s">
-        <v>96</v>
+      <c r="M72" s="14" t="str">
+        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <v>$/h/kW</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B73" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C73" s="20"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="18"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M73" s="14" t="str">
+        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <v>$/h/kW</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B74" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C74" s="20"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="18"/>
+      <c r="K74" s="14"/>
+      <c r="L74" s="14">
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="M74" s="14" t="str">
+        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <v>$/h/kW</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B75" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C75" s="20"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="18"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="M75" s="14" t="str">
+        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <v>$/h/kW</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Right path on data/
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_pypsa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Library/Group Containers/G69SCX94XU.duck/Library/Application Support/duck/Volumes.noindex/DPB-DGE Data Transfer Node/nobackup/scratch/awongel/clab_pypsa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD98C95-54D5-0849-9963-80C85B3DF19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADF4961-E8C8-3041-A0E0-08B97853B78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="500" windowWidth="27920" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,7 +353,7 @@
     <t>test_case</t>
   </si>
   <si>
-    <t>/carnegie/data/Shared/Labs/Caldeira\ Lab/Everyone/energy_demand_capacity_data/test_case_solar_wind_demand/</t>
+    <t>/carnegie/data/Shared/Labs/Caldeira Lab/Everyone/energy_demand_capacity_data/test_case_solar_wind_demand/</t>
   </si>
 </sst>
 </file>
@@ -889,7 +889,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -926,7 +926,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1286,7 +1285,7 @@
   <dimension ref="A1:S76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1539,7 +1538,7 @@
       <c r="A25" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1598,7 +1597,7 @@
       <c r="C31" s="10"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="22" t="s">
+      <c r="A32" t="s">
         <v>99</v>
       </c>
       <c r="B32" s="21">
@@ -1610,7 +1609,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" s="22" t="s">
+      <c r="A33" t="s">
         <v>100</v>
       </c>
       <c r="B33" s="21">

</xml_diff>

<commit_message>
Include some updates in case input file
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Library/Group Containers/G69SCX94XU.duck/Library/Application Support/duck/Volumes.noindex/DPB-DGE Data Transfer Node/nobackup/scratch/awongel/clab_pypsa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_pypsa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADF4961-E8C8-3041-A0E0-08B97853B78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F836BA01-8361-8C4A-8DB6-C57AFE73745A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="500" windowWidth="27920" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="880" windowWidth="28500" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_intermodel_one_node_" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="111">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -354,6 +354,18 @@
   </si>
   <si>
     <t>/carnegie/data/Shared/Labs/Caldeira Lab/Everyone/energy_demand_capacity_data/test_case_solar_wind_demand/</t>
+  </si>
+  <si>
+    <t>costs_path</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/PyPSA/technology-data/master/outputs/costs_2020.csv</t>
+  </si>
+  <si>
+    <t>p_min_pu</t>
+  </si>
+  <si>
+    <t>Note: p_min_pu allow bidirectionality of link</t>
   </si>
 </sst>
 </file>
@@ -363,7 +375,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,6 +522,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="36">
@@ -889,7 +908,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -927,6 +946,8 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1282,9 +1303,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S76"/>
+  <dimension ref="A1:T77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -1544,840 +1565,833 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
+        <v>107</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C30" s="8"/>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" s="10"/>
+        <v>43</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="21">
-        <f>(B30-B29)*24/B31</f>
+      <c r="B33" s="21">
+        <f>(B31-B30)*24/B32</f>
         <v>8784</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>100</v>
       </c>
-      <c r="B33" s="21">
-        <f>B32*B31</f>
+      <c r="B34" s="21">
+        <f>B33*B32</f>
         <v>8784</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" t="s">
+      <c r="C36" s="7"/>
+      <c r="D36" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B37" s="1">
         <v>10000000000</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" t="s">
+      <c r="C37" s="1"/>
+      <c r="D37" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="F42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>18</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I43" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D43" t="s">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
         <v>76</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H44" t="s">
         <v>83</v>
       </c>
-      <c r="O43" t="s">
+      <c r="O44" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+    <row r="45" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+    <row r="46" spans="1:18" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="H46" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="I46" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="J46" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="L46" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M45" s="4" t="s">
+      <c r="N46" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O45" s="5" t="s">
+      <c r="P46" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5" t="s">
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:18" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F48" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="J48" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="L48" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M47" s="2" t="s">
+      <c r="N48" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N47" s="2" t="s">
+      <c r="O48" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O47" s="2" t="s">
+      <c r="P48" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P47" s="2" t="s">
+      <c r="Q48" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Q47" s="2" t="s">
+      <c r="R48" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>28</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>28</v>
-      </c>
-      <c r="D48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F48" t="s">
-        <v>50</v>
-      </c>
-      <c r="I48" s="21">
-        <f>L68*B33</f>
-        <v>171.65443408509168</v>
-      </c>
-      <c r="J48" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
-        <v>$/time range/kW</v>
-      </c>
-      <c r="K48" s="15"/>
-      <c r="L48" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
-        <v>$/kWh</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B49" t="s">
-        <v>19</v>
-      </c>
-      <c r="C49" t="s">
-        <v>19</v>
       </c>
       <c r="D49" t="s">
         <v>22</v>
       </c>
-      <c r="F49" t="s">
-        <v>51</v>
-      </c>
-      <c r="I49" s="15"/>
-      <c r="K49" s="15"/>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>50</v>
+      </c>
+      <c r="J49" s="21">
+        <f>L69*B34</f>
+        <v>171.65443408509168</v>
+      </c>
+      <c r="K49" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
+        <v>$/time range/kW</v>
+      </c>
+      <c r="L49" s="15"/>
+      <c r="M49" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <v>$/kWh</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D50" t="s">
         <v>22</v>
       </c>
-      <c r="I50" s="21">
-        <f>L69*B33</f>
-        <v>104.08824719790415</v>
-      </c>
-      <c r="J50" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
-        <v>$/time range/kW</v>
-      </c>
-      <c r="K50" s="15">
-        <f>H69 + I69/J69</f>
-        <v>3.9088110924995347E-2</v>
-      </c>
-      <c r="L50" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
-        <v>$/kWh</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G50" t="s">
+        <v>51</v>
+      </c>
+      <c r="J50" s="15"/>
+      <c r="L50" s="15"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
       </c>
-      <c r="I51" s="21">
-        <f>L70*M51*B33</f>
-        <v>223.87212597208145</v>
-      </c>
-      <c r="J51" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
+      <c r="J51" s="21">
+        <f>L70*B34</f>
+        <v>104.08824719790415</v>
+      </c>
+      <c r="K51" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K51" s="15"/>
-      <c r="L51" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+      <c r="L51" s="15">
+        <f>H70 + I70/J70</f>
+        <v>3.9088110924995347E-2</v>
+      </c>
+      <c r="M51" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
         <v>$/kWh</v>
       </c>
-      <c r="M51">
-        <v>6.008</v>
-      </c>
-      <c r="N51" t="b">
-        <v>1</v>
-      </c>
-      <c r="O51">
-        <v>0.9</v>
-      </c>
-      <c r="Q51">
-        <v>1.1400000000000001E-6</v>
-      </c>
-      <c r="R51" t="str">
-        <f xml:space="preserve"> 1 &amp; "/" &amp; B38</f>
-        <v>1/h</v>
-      </c>
-      <c r="S51" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B52" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D52" t="s">
         <v>22</v>
       </c>
-      <c r="I52" s="21">
-        <f>L71*B33</f>
-        <v>548.78374889246641</v>
-      </c>
-      <c r="J52" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
+      <c r="J52" s="21">
+        <f>L71*N52*B34</f>
+        <v>223.87212597208145</v>
+      </c>
+      <c r="K52" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K52" s="15">
-        <f>H71 + I71/J71</f>
-        <v>2.5047272727272724E-2</v>
-      </c>
-      <c r="L52" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+      <c r="L52" s="15"/>
+      <c r="M52" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
         <v>$/kWh</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="N52">
+        <v>6.008</v>
+      </c>
+      <c r="O52" t="b">
+        <v>1</v>
+      </c>
+      <c r="P52">
+        <v>0.9</v>
+      </c>
+      <c r="R52">
+        <v>1.1400000000000001E-6</v>
+      </c>
+      <c r="S52" t="str">
+        <f xml:space="preserve"> 1 &amp; "/" &amp; B39</f>
+        <v>1/h</v>
+      </c>
+      <c r="T52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
       </c>
-      <c r="F53" t="s">
-        <v>52</v>
-      </c>
-      <c r="I53" s="21">
-        <f>L72*B33</f>
-        <v>181.49756560590552</v>
-      </c>
-      <c r="J53" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
+      <c r="J53" s="21">
+        <f>L72*B34</f>
+        <v>548.78374889246641</v>
+      </c>
+      <c r="K53" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K53" s="15"/>
-      <c r="L53" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+      <c r="L53" s="15">
+        <f>H72 + I72/J72</f>
+        <v>2.5047272727272724E-2</v>
+      </c>
+      <c r="M53" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C54" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D54" t="s">
         <v>22</v>
       </c>
-      <c r="E54" t="s">
+      <c r="G54" t="s">
+        <v>52</v>
+      </c>
+      <c r="J54" s="21">
+        <f>L73*B34</f>
+        <v>181.49756560590552</v>
+      </c>
+      <c r="K54" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
+        <v>$/time range/kW</v>
+      </c>
+      <c r="L54" s="15"/>
+      <c r="M54" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <v>$/kWh</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55" t="s">
         <v>38</v>
       </c>
-      <c r="I54" s="21">
-        <f>L73*B33</f>
+      <c r="J55" s="21">
+        <f>L74*B34</f>
         <v>43.92</v>
       </c>
-      <c r="J54" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
+      <c r="K55" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K54" s="15"/>
-      <c r="L54" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+      <c r="L55" s="15"/>
+      <c r="M55" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
         <v>$/kWh</v>
       </c>
-      <c r="O54">
+      <c r="P55">
         <v>0.7</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>39</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>39</v>
-      </c>
-      <c r="D55" t="s">
-        <v>38</v>
-      </c>
-      <c r="I55" s="21">
-        <f>L74*B33</f>
-        <v>0.140544</v>
-      </c>
-      <c r="J55" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39 &amp; B38</f>
-        <v>$/time range/kWh</v>
-      </c>
-      <c r="K55" s="15"/>
-      <c r="L55" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
-        <v>$/kWh</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B56" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56" t="s">
-        <v>40</v>
       </c>
       <c r="D56" t="s">
         <v>38</v>
       </c>
-      <c r="E56" t="s">
+      <c r="J56" s="21">
+        <f>L75*B34</f>
+        <v>0.140544</v>
+      </c>
+      <c r="K56" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40 &amp; B39</f>
+        <v>$/time range/kWh</v>
+      </c>
+      <c r="L56" s="15"/>
+      <c r="M56" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <v>$/kWh</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B57" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" t="s">
         <v>22</v>
       </c>
-      <c r="I56" s="21">
-        <f>L75*B33</f>
+      <c r="J57" s="21">
+        <f>L76*B34</f>
         <v>17.568000000000001</v>
       </c>
-      <c r="J56" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
+      <c r="K57" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K56" s="15"/>
-      <c r="L56" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+      <c r="L57" s="15"/>
+      <c r="M57" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
         <v>$/kWh</v>
       </c>
-      <c r="O56">
+      <c r="P57">
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A62" s="15" t="s">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A63" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>89</v>
-      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A65" s="12" t="s">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>89</v>
+      </c>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="11"/>
-      <c r="L65" s="2"/>
-      <c r="M65" s="2"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A66" s="12"/>
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="11"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" s="12"/>
+      <c r="B67" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C66" s="14">
+      <c r="C67" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
-      <c r="I66" s="16"/>
-      <c r="J66" s="16"/>
-      <c r="K66" s="16"/>
-      <c r="L66" s="16"/>
-      <c r="M66" s="16"/>
-    </row>
-    <row r="67" spans="1:13" ht="64" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
-      <c r="B67" s="13" t="s">
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="16"/>
+      <c r="L67" s="16"/>
+      <c r="M67" s="16"/>
+    </row>
+    <row r="68" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A68" s="2"/>
+      <c r="B68" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C67" s="19" t="str">
-        <f xml:space="preserve"> "Overnight cost [" &amp; B40 &amp; "/" &amp; B39 &amp; "]"</f>
+      <c r="C68" s="19" t="str">
+        <f xml:space="preserve"> "Overnight cost [" &amp; B41 &amp; "/" &amp; B40 &amp; "]"</f>
         <v>Overnight cost [$/kW]</v>
       </c>
-      <c r="D67" s="13" t="str">
-        <f xml:space="preserve"> "Fixed O&amp;M cost ["  &amp; B40 &amp; "/" &amp; B39 &amp; "year]"</f>
+      <c r="D68" s="13" t="str">
+        <f xml:space="preserve"> "Fixed O&amp;M cost ["  &amp; B41 &amp; "/" &amp; B40 &amp; "year]"</f>
         <v>Fixed O&amp;M cost [$/kWyear]</v>
       </c>
-      <c r="E67" s="13" t="s">
+      <c r="E68" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F67" s="13" t="s">
+      <c r="F68" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="G67" s="17" t="str">
-        <f xml:space="preserve"> "Annual fixed costs [" &amp;B40 &amp; "/year]"</f>
+      <c r="G68" s="17" t="str">
+        <f xml:space="preserve"> "Annual fixed costs [" &amp;B41 &amp; "/year]"</f>
         <v>Annual fixed costs [$/year]</v>
       </c>
-      <c r="H67" s="13" t="str">
-        <f xml:space="preserve"> "Variable O&amp;M [" &amp; B40 &amp; "/" &amp; B39 &amp; B38 &amp; "]"</f>
+      <c r="H68" s="13" t="str">
+        <f xml:space="preserve"> "Variable O&amp;M [" &amp; B41 &amp; "/" &amp; B40 &amp; B39 &amp; "]"</f>
         <v>Variable O&amp;M [$/kWh]</v>
       </c>
-      <c r="I67" s="13" t="str">
-        <f xml:space="preserve"> "Fuel cost [" &amp; B40 &amp; "/" &amp; B39 &amp; B38 &amp; "]"</f>
+      <c r="I68" s="13" t="str">
+        <f xml:space="preserve"> "Fuel cost [" &amp; B41 &amp; "/" &amp; B40 &amp; B39 &amp; "]"</f>
         <v>Fuel cost [$/kWh]</v>
       </c>
-      <c r="J67" s="13" t="s">
+      <c r="J68" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="K67" s="19"/>
-      <c r="L67" s="13" t="s">
+      <c r="K68" s="19"/>
+      <c r="L68" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="M67" s="13"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B68" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C68" s="20">
-        <v>1851</v>
-      </c>
-      <c r="D68" s="14">
-        <v>22.02</v>
-      </c>
-      <c r="E68" s="14">
-        <f>C66*(1+C66)^F68/((1+C66)^F68-1)</f>
-        <v>8.0586403511111196E-2</v>
-      </c>
-      <c r="F68" s="14">
-        <v>30</v>
-      </c>
-      <c r="G68" s="18">
-        <f>C68*E68+D68</f>
-        <v>171.18543289906683</v>
-      </c>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
-      <c r="K68" s="20"/>
-      <c r="L68" s="14">
-        <f>G68/8760</f>
-        <v>1.954171608436836E-2</v>
-      </c>
-      <c r="M68" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
-        <v>$/h/kW</v>
-      </c>
+      <c r="M68" s="13"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B69" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C69" s="20">
-        <v>982</v>
+        <v>1851</v>
       </c>
       <c r="D69" s="14">
-        <v>11.11</v>
+        <v>22.02</v>
       </c>
       <c r="E69" s="14">
-        <f>C66*(1+C66)^F69/((1+C66)^F69-1)</f>
-        <v>9.4392925743255696E-2</v>
+        <f>C67*(1+C67)^F69/((1+C67)^F69-1)</f>
+        <v>8.0586403511111196E-2</v>
       </c>
       <c r="F69" s="14">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G69" s="18">
         <f>C69*E69+D69</f>
-        <v>103.80385307987709</v>
-      </c>
-      <c r="H69" s="14">
-        <v>3.5400000000000002E-3</v>
-      </c>
-      <c r="I69" s="14">
-        <v>1.9099999999999999E-2</v>
-      </c>
-      <c r="J69" s="14">
-        <v>0.5373</v>
-      </c>
+        <v>171.18543289906683</v>
+      </c>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
       <c r="K69" s="20"/>
       <c r="L69" s="14">
         <f>G69/8760</f>
-        <v>1.1849754917794188E-2</v>
+        <v>1.954171608436836E-2</v>
       </c>
       <c r="M69" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B70" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C70" s="20">
-        <v>261</v>
-      </c>
-      <c r="D70" s="14"/>
+        <v>982</v>
+      </c>
+      <c r="D70" s="14">
+        <v>11.11</v>
+      </c>
       <c r="E70" s="14">
-        <f>C66*(1+C66)^F70/((1+C66)^F70-1)</f>
-        <v>0.14237750272736471</v>
+        <f>C67*(1+C67)^F70/((1+C67)^F70-1)</f>
+        <v>9.4392925743255696E-2</v>
       </c>
       <c r="F70" s="14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G70" s="18">
         <f>C70*E70+D70</f>
-        <v>37.160528211842191</v>
-      </c>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
+        <v>103.80385307987709</v>
+      </c>
+      <c r="H70" s="14">
+        <v>3.5400000000000002E-3</v>
+      </c>
+      <c r="I70" s="14">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="J70" s="14">
+        <v>0.5373</v>
+      </c>
       <c r="K70" s="20"/>
       <c r="L70" s="14">
         <f>G70/8760</f>
-        <v>4.2420694305755928E-3</v>
+        <v>1.1849754917794188E-2</v>
       </c>
       <c r="M70" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B71" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C71" s="20">
-        <v>5946</v>
-      </c>
-      <c r="D71" s="14">
-        <v>101.28</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="D71" s="14"/>
       <c r="E71" s="14">
-        <f>C66*(1+C66)^F71/((1+C66)^F71-1)</f>
-        <v>7.5009138873610326E-2</v>
+        <f>C67*(1+C67)^F71/((1+C67)^F71-1)</f>
+        <v>0.14237750272736471</v>
       </c>
       <c r="F71" s="14">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G71" s="18">
         <f>C71*E71+D71</f>
-        <v>547.28433974248696</v>
-      </c>
-      <c r="H71" s="14">
-        <v>2.32E-3</v>
-      </c>
-      <c r="I71" s="14">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="J71" s="14">
-        <v>0.33</v>
-      </c>
+        <v>37.160528211842191</v>
+      </c>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
       <c r="K71" s="20"/>
       <c r="L71" s="14">
         <f>G71/8760</f>
-        <v>6.2475381249142349E-2</v>
+        <v>4.2420694305755928E-3</v>
       </c>
       <c r="M71" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B72" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C72" s="20">
-        <v>1657</v>
+        <v>5946</v>
       </c>
       <c r="D72" s="14">
-        <v>47.47</v>
+        <v>101.28</v>
       </c>
       <c r="E72" s="14">
-        <f>C66*(1+C66)^F72/((1+C66)^F72-1)</f>
-        <v>8.0586403511111196E-2</v>
+        <f>C67*(1+C67)^F72/((1+C67)^F72-1)</f>
+        <v>7.5009138873610326E-2</v>
       </c>
       <c r="F72" s="14">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G72" s="18">
         <f>C72*E72+D72</f>
-        <v>181.00167061791126</v>
-      </c>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
+        <v>547.28433974248696</v>
+      </c>
+      <c r="H72" s="14">
+        <v>2.32E-3</v>
+      </c>
+      <c r="I72" s="14">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="J72" s="14">
+        <v>0.33</v>
+      </c>
       <c r="K72" s="20"/>
       <c r="L72" s="14">
         <f>G72/8760</f>
-        <v>2.0662291166428225E-2</v>
+        <v>6.2475381249142349E-2</v>
       </c>
       <c r="M72" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B73" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C73" s="20"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="18"/>
+        <v>34</v>
+      </c>
+      <c r="C73" s="20">
+        <v>1657</v>
+      </c>
+      <c r="D73" s="14">
+        <v>47.47</v>
+      </c>
+      <c r="E73" s="14">
+        <f>C67*(1+C67)^F73/((1+C67)^F73-1)</f>
+        <v>8.0586403511111196E-2</v>
+      </c>
+      <c r="F73" s="14">
+        <v>30</v>
+      </c>
+      <c r="G73" s="18">
+        <f>C73*E73+D73</f>
+        <v>181.00167061791126</v>
+      </c>
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
-      <c r="J73" s="18"/>
-      <c r="K73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="20"/>
       <c r="L73" s="14">
-        <v>5.0000000000000001E-3</v>
+        <f>G73/8760</f>
+        <v>2.0662291166428225E-2</v>
       </c>
       <c r="M73" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B74" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C74" s="20"/>
       <c r="D74" s="14"/>
@@ -2389,16 +2403,16 @@
       <c r="J74" s="18"/>
       <c r="K74" s="14"/>
       <c r="L74" s="14">
-        <v>1.5999999999999999E-5</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="M74" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B75" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C75" s="20"/>
       <c r="D75" s="14"/>
@@ -2410,15 +2424,36 @@
       <c r="J75" s="18"/>
       <c r="K75" s="14"/>
       <c r="L75" s="14">
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="M75" s="14" t="str">
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
+        <v>$/h/kW</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B76" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C76" s="20"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="18"/>
+      <c r="K76" s="14"/>
+      <c r="L76" s="14">
         <v>2E-3</v>
       </c>
-      <c r="M75" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+      <c r="M76" s="14" t="str">
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B76" t="s">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>